<commit_message>
택5 -> 택 1
</commit_message>
<xml_diff>
--- a/Z3 Solver/GraduationRequirement/GraduationRequirements2023.xlsx
+++ b/Z3 Solver/GraduationRequirement/GraduationRequirements2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eeheu\Downloads\z3\grad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BDAC90-6E1D-4EF2-AE66-DBC94CCB0E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D363A675-2796-4B2B-9A0F-5251F3DEFFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="1290" windowWidth="16515" windowHeight="13230" xr2:uid="{2A619A1B-6C3E-4E95-A24C-5272A029B6E8}"/>
+    <workbookView xWindow="40800" yWindow="-765" windowWidth="16515" windowHeight="13230" xr2:uid="{2A619A1B-6C3E-4E95-A24C-5272A029B6E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="108">
   <si>
     <t>전공필수</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,10 +421,6 @@
   </si>
   <si>
     <t>필수</t>
-  </si>
-  <si>
-    <t>택5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>택3</t>
@@ -842,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892549DD-7741-4CD4-804D-2EE94914B9F6}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1058,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1203,7 +1199,7 @@
         <v>87</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1220,7 +1216,7 @@
         <v>88</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1237,7 +1233,7 @@
         <v>89</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1254,7 +1250,7 @@
         <v>90</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1271,7 +1267,7 @@
         <v>91</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1288,7 +1284,7 @@
         <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1305,7 +1301,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1322,7 +1318,7 @@
         <v>30</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1339,7 +1335,7 @@
         <v>36</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1356,7 +1352,7 @@
         <v>35</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1373,7 +1369,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1458,7 +1454,7 @@
         <v>49</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1475,7 +1471,7 @@
         <v>51</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1492,7 +1488,7 @@
         <v>45</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1509,7 +1505,7 @@
         <v>55</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1526,7 +1522,7 @@
         <v>57</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1543,7 +1539,7 @@
         <v>59</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>